<commit_message>
updating starwars.xlsx to include exercise 6
</commit_message>
<xml_diff>
--- a/E1_starwars.xlsx
+++ b/E1_starwars.xlsx
@@ -8,17 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EpicWork\workspace\excel\individual-projects\exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F0FA49-477A-4F9E-AF3B-CB40F0BA72CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9F39B5-336F-460D-AA6E-271628DFACB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4665" yWindow="4365" windowWidth="19905" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="90" yWindow="60" windowWidth="19905" windowHeight="16200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="starwars" sheetId="1" r:id="rId1"/>
-    <sheet name="data_dictionary" sheetId="2" r:id="rId2"/>
-    <sheet name="Answers" sheetId="3" r:id="rId3"/>
+    <sheet name="height_filter" sheetId="4" r:id="rId2"/>
+    <sheet name="data_dictionary" sheetId="2" r:id="rId3"/>
+    <sheet name="Answers" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">starwars!$D$1:$D$96</definedName>
     <definedName name="BMI">starwars!$G$2:$G$88</definedName>
+    <definedName name="height_data">height_filter!$C$2:$C$82</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,8 +40,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="295">
   <si>
     <t>name</t>
   </si>
@@ -881,12 +906,57 @@
   </si>
   <si>
     <t>weight(lbs)</t>
+  </si>
+  <si>
+    <t>Mean height:</t>
+  </si>
+  <si>
+    <t>Mode height:</t>
+  </si>
+  <si>
+    <t>height_order</t>
+  </si>
+  <si>
+    <t>Midpoint:</t>
+  </si>
+  <si>
+    <t>Median height:</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>Functions</t>
+  </si>
+  <si>
+    <t>diff_mean</t>
+  </si>
+  <si>
+    <t>diff_mean_sqd</t>
+  </si>
+  <si>
+    <t>Variance:</t>
+  </si>
+  <si>
+    <t>Standard Deviation:</t>
+  </si>
+  <si>
+    <t>90th Percentile:</t>
+  </si>
+  <si>
+    <t>25th Percentile:</t>
+  </si>
+  <si>
+    <t>Rank:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1381,7 +1451,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1389,6 +1459,7 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1434,7 +1505,38 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1746,8 +1848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F88"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1883,7 +1985,7 @@
       </c>
       <c r="P2" s="6">
         <f ca="1">IF(O2="NA", "NA", TODAY()-O2)</f>
-        <v>39100</v>
+        <v>39101</v>
       </c>
       <c r="Q2" t="s">
         <v>14</v>
@@ -1955,7 +2057,7 @@
       </c>
       <c r="P3" s="6">
         <f t="shared" ref="P3:P66" ca="1" si="9">IF(O3="NA", "NA", TODAY()-O3)</f>
-        <v>5155</v>
+        <v>5156</v>
       </c>
       <c r="Q3" t="s">
         <v>14</v>
@@ -2027,7 +2129,7 @@
       </c>
       <c r="P4" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>33990</v>
+        <v>33991</v>
       </c>
       <c r="Q4" t="s">
         <v>26</v>
@@ -2099,7 +2201,7 @@
       </c>
       <c r="P5" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>30741.5</v>
+        <v>30742.5</v>
       </c>
       <c r="Q5" t="s">
         <v>14</v>
@@ -2171,7 +2273,7 @@
       </c>
       <c r="P6" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>39100</v>
+        <v>39101</v>
       </c>
       <c r="Q6" t="s">
         <v>35</v>
@@ -2243,7 +2345,7 @@
       </c>
       <c r="P7" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>27055</v>
+        <v>27056</v>
       </c>
       <c r="Q7" t="s">
         <v>14</v>
@@ -2315,7 +2417,7 @@
       </c>
       <c r="P8" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>28880</v>
+        <v>28881</v>
       </c>
       <c r="Q8" t="s">
         <v>14</v>
@@ -2459,7 +2561,7 @@
       </c>
       <c r="P10" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>37275</v>
+        <v>37276</v>
       </c>
       <c r="Q10" t="s">
         <v>14</v>
@@ -2531,7 +2633,7 @@
       </c>
       <c r="P11" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>25230</v>
+        <v>25231</v>
       </c>
       <c r="Q11" t="s">
         <v>49</v>
@@ -2603,7 +2705,7 @@
       </c>
       <c r="P12" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>30741.5</v>
+        <v>30742.5</v>
       </c>
       <c r="Q12" t="s">
         <v>14</v>
@@ -2675,7 +2777,7 @@
       </c>
       <c r="P13" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>22675</v>
+        <v>22676</v>
       </c>
       <c r="Q13" t="s">
         <v>54</v>
@@ -2747,7 +2849,7 @@
       </c>
       <c r="P14" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>-26965</v>
+        <v>-26964</v>
       </c>
       <c r="Q14" t="s">
         <v>58</v>
@@ -2819,7 +2921,7 @@
       </c>
       <c r="P15" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>35450</v>
+        <v>35451</v>
       </c>
       <c r="Q15" t="s">
         <v>61</v>
@@ -2891,7 +2993,7 @@
       </c>
       <c r="P16" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>29975</v>
+        <v>29976</v>
       </c>
       <c r="Q16" t="s">
         <v>65</v>
@@ -2963,7 +3065,7 @@
       </c>
       <c r="P17" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>-172965</v>
+        <v>-172964</v>
       </c>
       <c r="Q17" t="s">
         <v>70</v>
@@ -3035,7 +3137,7 @@
       </c>
       <c r="P18" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>38370</v>
+        <v>38371</v>
       </c>
       <c r="Q18" t="s">
         <v>61</v>
@@ -3179,7 +3281,7 @@
       </c>
       <c r="P20" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>-281005</v>
+        <v>-281004</v>
       </c>
       <c r="Q20" t="s">
         <v>18</v>
@@ -3251,7 +3353,7 @@
       </c>
       <c r="P21" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>16105</v>
+        <v>16106</v>
       </c>
       <c r="Q21" t="s">
         <v>26</v>
@@ -3323,7 +3425,7 @@
       </c>
       <c r="P22" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>34537.5</v>
+        <v>34538.5</v>
       </c>
       <c r="Q22" t="s">
         <v>86</v>
@@ -3395,7 +3497,7 @@
       </c>
       <c r="P23" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>40560</v>
+        <v>40561</v>
       </c>
       <c r="Q23" t="s">
         <v>18</v>
@@ -3467,7 +3569,7 @@
       </c>
       <c r="P24" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>26690</v>
+        <v>26691</v>
       </c>
       <c r="Q24" t="s">
         <v>92</v>
@@ -3539,7 +3641,7 @@
       </c>
       <c r="P25" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>34720</v>
+        <v>34721</v>
       </c>
       <c r="Q25" t="s">
         <v>96</v>
@@ -3611,7 +3713,7 @@
       </c>
       <c r="P26" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>32530</v>
+        <v>32531</v>
       </c>
       <c r="Q26" t="s">
         <v>99</v>
@@ -3683,7 +3785,7 @@
       </c>
       <c r="P27" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>31070</v>
+        <v>31071</v>
       </c>
       <c r="Q27" t="s">
         <v>102</v>
@@ -3755,7 +3857,7 @@
       </c>
       <c r="P28" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>28515</v>
+        <v>28516</v>
       </c>
       <c r="Q28" t="s">
         <v>107</v>
@@ -3899,7 +4001,7 @@
       </c>
       <c r="P30" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>43115</v>
+        <v>43116</v>
       </c>
       <c r="Q30" t="s">
         <v>111</v>
@@ -4043,7 +4145,7 @@
       </c>
       <c r="P32" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>12455</v>
+        <v>12456</v>
       </c>
       <c r="Q32" t="s">
         <v>18</v>
@@ -4187,7 +4289,7 @@
       </c>
       <c r="P34" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>12820</v>
+        <v>12821</v>
       </c>
       <c r="Q34" t="s">
         <v>123</v>
@@ -4259,7 +4361,7 @@
       </c>
       <c r="P35" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>27055</v>
+        <v>27056</v>
       </c>
       <c r="Q35" t="s">
         <v>26</v>
@@ -4691,7 +4793,7 @@
       </c>
       <c r="P41" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>23405</v>
+        <v>23406</v>
       </c>
       <c r="Q41" t="s">
         <v>26</v>
@@ -4763,7 +4865,7 @@
       </c>
       <c r="P42" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>19755</v>
+        <v>19756</v>
       </c>
       <c r="Q42" t="s">
         <v>14</v>
@@ -4835,7 +4937,7 @@
       </c>
       <c r="P43" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>26325</v>
+        <v>26326</v>
       </c>
       <c r="Q43" t="s">
         <v>142</v>
@@ -4979,7 +5081,7 @@
       </c>
       <c r="P45" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>28515</v>
+        <v>28516</v>
       </c>
       <c r="Q45" t="s">
         <v>146</v>
@@ -5267,7 +5369,7 @@
       </c>
       <c r="P49" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>19755</v>
+        <v>19756</v>
       </c>
       <c r="Q49" t="s">
         <v>161</v>
@@ -5339,7 +5441,7 @@
       </c>
       <c r="P50" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>12455</v>
+        <v>12456</v>
       </c>
       <c r="Q50" t="s">
         <v>163</v>
@@ -5771,7 +5873,7 @@
       </c>
       <c r="P56" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>38005</v>
+        <v>38006</v>
       </c>
       <c r="Q56" t="s">
         <v>180</v>
@@ -6059,7 +6161,7 @@
       </c>
       <c r="P60" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>16105</v>
+        <v>16106</v>
       </c>
       <c r="Q60" t="s">
         <v>14</v>
@@ -6203,7 +6305,7 @@
       </c>
       <c r="P62" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>24865</v>
+        <v>24866</v>
       </c>
       <c r="Q62" t="s">
         <v>194</v>
@@ -6275,7 +6377,7 @@
       </c>
       <c r="P63" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>31435</v>
+        <v>31436</v>
       </c>
       <c r="Q63" t="s">
         <v>194</v>
@@ -6419,7 +6521,7 @@
       </c>
       <c r="P65" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>8805</v>
+        <v>8806</v>
       </c>
       <c r="Q65" t="s">
         <v>199</v>
@@ -6462,7 +6564,7 @@
         <v>0</v>
       </c>
       <c r="H66" s="5">
-        <f t="shared" ref="H66:H97" si="12">RANK(G66, BMI)</f>
+        <f t="shared" ref="H66:H88" si="12">RANK(G66, BMI)</f>
         <v>60</v>
       </c>
       <c r="I66" s="3">
@@ -6491,7 +6593,7 @@
       </c>
       <c r="P66" s="6">
         <f t="shared" ca="1" si="9"/>
-        <v>21580</v>
+        <v>21581</v>
       </c>
       <c r="Q66" t="s">
         <v>35</v>
@@ -6563,7 +6665,7 @@
       </c>
       <c r="P67" s="6">
         <f t="shared" ref="P67:P88" ca="1" si="20">IF(O67="NA", "NA", TODAY()-O67)</f>
-        <v>21945</v>
+        <v>21946</v>
       </c>
       <c r="Q67" t="s">
         <v>203</v>
@@ -8075,7 +8177,7 @@
       </c>
       <c r="P88" s="6">
         <f t="shared" ca="1" si="20"/>
-        <v>29245</v>
+        <v>29246</v>
       </c>
       <c r="Q88" t="s">
         <v>26</v>
@@ -8100,6 +8202,1714 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E919E3-E024-4A3D-8E89-7053258A8778}">
+  <dimension ref="A1:J82"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" customWidth="1"/>
+    <col min="5" max="5" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str" cm="1">
+        <f t="array" ref="B2:C82">_xlfn._xlws.SORT(_xlfn._xlws.FILTER(starwars!A2:B88,ISNUMBER(starwars!B2:B88)),2)</f>
+        <v>Yoda</v>
+      </c>
+      <c r="C2">
+        <v>66</v>
+      </c>
+      <c r="D2" s="7">
+        <f>$H$12-$C2</f>
+        <v>108.35802469135803</v>
+      </c>
+      <c r="E2" s="7">
+        <f>$D2^2</f>
+        <v>11741.461515012956</v>
+      </c>
+      <c r="G2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Ratts Tyerell</v>
+      </c>
+      <c r="C3">
+        <v>79</v>
+      </c>
+      <c r="D3" s="7">
+        <f>$H$12-$C3</f>
+        <v>95.358024691358025</v>
+      </c>
+      <c r="E3" s="7">
+        <f t="shared" ref="E3:E66" si="0">$D3^2</f>
+        <v>9093.1528730376467</v>
+      </c>
+      <c r="G3" t="s">
+        <v>281</v>
+      </c>
+      <c r="H3">
+        <f>SUM(height_data)/COUNT(height_data)</f>
+        <v>174.35802469135803</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Wicket Systri Warrick</v>
+      </c>
+      <c r="C4">
+        <v>88</v>
+      </c>
+      <c r="D4" s="7">
+        <f>$H$12-$C4</f>
+        <v>86.358024691358025</v>
+      </c>
+      <c r="E4" s="7">
+        <f t="shared" si="0"/>
+        <v>7457.7084285932024</v>
+      </c>
+      <c r="G4" t="s">
+        <v>285</v>
+      </c>
+      <c r="H4">
+        <f>(VLOOKUP(40, A2:C82, 3, FALSE) + VLOOKUP(41, A2:C82, 3, FALSE))/2</f>
+        <v>180</v>
+      </c>
+      <c r="I4" t="s">
+        <v>284</v>
+      </c>
+      <c r="J4">
+        <f>COUNT(height_data)/2</f>
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Dud Bolt</v>
+      </c>
+      <c r="C5">
+        <v>94</v>
+      </c>
+      <c r="D5" s="7">
+        <f>$H$12-$C5</f>
+        <v>80.358024691358025</v>
+      </c>
+      <c r="E5" s="7">
+        <f t="shared" si="0"/>
+        <v>6457.4121322969058</v>
+      </c>
+      <c r="G5" t="s">
+        <v>282</v>
+      </c>
+      <c r="H5">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <v>R2-D2</v>
+      </c>
+      <c r="C6">
+        <v>96</v>
+      </c>
+      <c r="D6" s="7">
+        <f>$H$12-$C6</f>
+        <v>78.358024691358025</v>
+      </c>
+      <c r="E6" s="7">
+        <f t="shared" si="0"/>
+        <v>6139.980033531474</v>
+      </c>
+      <c r="G6" t="s">
+        <v>290</v>
+      </c>
+      <c r="H6" s="7">
+        <f>AVERAGE(E2:E82)</f>
+        <v>1194.0570035055634</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <v>R4-P17</v>
+      </c>
+      <c r="C7">
+        <v>96</v>
+      </c>
+      <c r="D7" s="7">
+        <f>$H$12-$C7</f>
+        <v>78.358024691358025</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="0"/>
+        <v>6139.980033531474</v>
+      </c>
+      <c r="G7" t="s">
+        <v>291</v>
+      </c>
+      <c r="H7">
+        <f>SQRT(H6)</f>
+        <v>34.555129915912104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <v>R5-D4</v>
+      </c>
+      <c r="C8">
+        <v>97</v>
+      </c>
+      <c r="D8" s="7">
+        <f>$H$12-$C8</f>
+        <v>77.358024691358025</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="0"/>
+        <v>5984.263984148758</v>
+      </c>
+      <c r="G8" t="s">
+        <v>292</v>
+      </c>
+      <c r="H8">
+        <f>VLOOKUP($J8, $A$2:$C$82, 3, FALSE)</f>
+        <v>206</v>
+      </c>
+      <c r="I8" t="s">
+        <v>294</v>
+      </c>
+      <c r="J8">
+        <f>_xlfn.CEILING.MATH(COUNT(height_data)*0.9)</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Sebulba</v>
+      </c>
+      <c r="C9">
+        <v>112</v>
+      </c>
+      <c r="D9" s="7">
+        <f>$H$12-$C9</f>
+        <v>62.358024691358025</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" si="0"/>
+        <v>3888.5232434080172</v>
+      </c>
+      <c r="G9" t="s">
+        <v>293</v>
+      </c>
+      <c r="H9">
+        <f>VLOOKUP($J9, $A$2:$C$82, 3, FALSE)</f>
+        <v>167</v>
+      </c>
+      <c r="I9" t="s">
+        <v>294</v>
+      </c>
+      <c r="J9">
+        <f>_xlfn.CEILING.MATH(COUNT(height_data)*0.25)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Gasgano</v>
+      </c>
+      <c r="C10">
+        <v>122</v>
+      </c>
+      <c r="D10" s="7">
+        <f>$H$12-$C10</f>
+        <v>52.358024691358025</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="0"/>
+        <v>2741.3627495808569</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Watto</v>
+      </c>
+      <c r="C11">
+        <v>137</v>
+      </c>
+      <c r="D11" s="7">
+        <f>$H$12-$C11</f>
+        <v>37.358024691358025</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="0"/>
+        <v>1395.622008840116</v>
+      </c>
+      <c r="G11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Leia Organa</v>
+      </c>
+      <c r="C12">
+        <v>150</v>
+      </c>
+      <c r="D12" s="7">
+        <f>$H$12-$C12</f>
+        <v>24.358024691358025</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="0"/>
+        <v>593.31336686480722</v>
+      </c>
+      <c r="G12" t="s">
+        <v>281</v>
+      </c>
+      <c r="H12" s="7">
+        <f>AVERAGE(height_data)</f>
+        <v>174.35802469135803</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Mon Mothma</v>
+      </c>
+      <c r="C13">
+        <v>150</v>
+      </c>
+      <c r="D13" s="7">
+        <f>$H$12-$C13</f>
+        <v>24.358024691358025</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="0"/>
+        <v>593.31336686480722</v>
+      </c>
+      <c r="G13" t="s">
+        <v>285</v>
+      </c>
+      <c r="H13">
+        <f>MEDIAN(height_data)</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Cordé</v>
+      </c>
+      <c r="C14">
+        <v>157</v>
+      </c>
+      <c r="D14" s="7">
+        <f>$H$12-$C14</f>
+        <v>17.358024691358025</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="0"/>
+        <v>301.30102118579487</v>
+      </c>
+      <c r="G14" t="s">
+        <v>282</v>
+      </c>
+      <c r="H14">
+        <f>_xlfn.MODE.SNGL(height_data)</f>
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Nien Nunb</v>
+      </c>
+      <c r="C15">
+        <v>160</v>
+      </c>
+      <c r="D15" s="7">
+        <f>$H$12-$C15</f>
+        <v>14.358024691358025</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="0"/>
+        <v>206.15287303764671</v>
+      </c>
+      <c r="G15" t="s">
+        <v>290</v>
+      </c>
+      <c r="H15">
+        <f>_xlfn.VAR.P(height_data)</f>
+        <v>1194.0570035055632</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Shmi Skywalker</v>
+      </c>
+      <c r="C16">
+        <v>163</v>
+      </c>
+      <c r="D16" s="7">
+        <f>$H$12-$C16</f>
+        <v>11.358024691358025</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="0"/>
+        <v>129.00472488949856</v>
+      </c>
+      <c r="G16" t="s">
+        <v>291</v>
+      </c>
+      <c r="H16">
+        <f>_xlfn.STDEV.P(height_data)</f>
+        <v>34.555129915912097</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Ben Quadinaros</v>
+      </c>
+      <c r="C17">
+        <v>163</v>
+      </c>
+      <c r="D17" s="7">
+        <f>$H$12-$C17</f>
+        <v>11.358024691358025</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" si="0"/>
+        <v>129.00472488949856</v>
+      </c>
+      <c r="G17" t="s">
+        <v>292</v>
+      </c>
+      <c r="H17">
+        <f>_xlfn.PERCENTILE.INC(height_data, 0.9)</f>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Beru Whitesun lars</v>
+      </c>
+      <c r="C18">
+        <v>165</v>
+      </c>
+      <c r="D18" s="7">
+        <f>$H$12-$C18</f>
+        <v>9.3580246913580254</v>
+      </c>
+      <c r="E18" s="7">
+        <f t="shared" si="0"/>
+        <v>87.57262612406646</v>
+      </c>
+      <c r="G18" t="s">
+        <v>293</v>
+      </c>
+      <c r="H18">
+        <f>_xlfn.QUARTILE.INC(height_data, 1)</f>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Dormé</v>
+      </c>
+      <c r="C19">
+        <v>165</v>
+      </c>
+      <c r="D19" s="7">
+        <f>$H$12-$C19</f>
+        <v>9.3580246913580254</v>
+      </c>
+      <c r="E19" s="7">
+        <f t="shared" si="0"/>
+        <v>87.57262612406646</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Padmé Amidala</v>
+      </c>
+      <c r="C20">
+        <v>165</v>
+      </c>
+      <c r="D20" s="7">
+        <f>$H$12-$C20</f>
+        <v>9.3580246913580254</v>
+      </c>
+      <c r="E20" s="7">
+        <f t="shared" si="0"/>
+        <v>87.57262612406646</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Barriss Offee</v>
+      </c>
+      <c r="C21">
+        <v>166</v>
+      </c>
+      <c r="D21" s="7">
+        <f>$H$12-$C21</f>
+        <v>8.3580246913580254</v>
+      </c>
+      <c r="E21" s="7">
+        <f t="shared" si="0"/>
+        <v>69.856576741350409</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="str">
+        <v>C-3PO</v>
+      </c>
+      <c r="C22">
+        <v>167</v>
+      </c>
+      <c r="D22" s="7">
+        <f>$H$12-$C22</f>
+        <v>7.3580246913580254</v>
+      </c>
+      <c r="E22" s="7">
+        <f t="shared" si="0"/>
+        <v>54.140527358634365</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Jocasta Nu</v>
+      </c>
+      <c r="C23">
+        <v>167</v>
+      </c>
+      <c r="D23" s="7">
+        <f>$H$12-$C23</f>
+        <v>7.3580246913580254</v>
+      </c>
+      <c r="E23" s="7">
+        <f t="shared" si="0"/>
+        <v>54.140527358634365</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Zam Wesell</v>
+      </c>
+      <c r="C24">
+        <v>168</v>
+      </c>
+      <c r="D24" s="7">
+        <f>$H$12-$C24</f>
+        <v>6.3580246913580254</v>
+      </c>
+      <c r="E24" s="7">
+        <f t="shared" si="0"/>
+        <v>40.424477975918315</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="str">
+        <v>Wedge Antilles</v>
+      </c>
+      <c r="C25">
+        <v>170</v>
+      </c>
+      <c r="D25" s="7">
+        <f>$H$12-$C25</f>
+        <v>4.3580246913580254</v>
+      </c>
+      <c r="E25" s="7">
+        <f t="shared" si="0"/>
+        <v>18.992379210486213</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="str">
+        <v>Palpatine</v>
+      </c>
+      <c r="C26">
+        <v>170</v>
+      </c>
+      <c r="D26" s="7">
+        <f>$H$12-$C26</f>
+        <v>4.3580246913580254</v>
+      </c>
+      <c r="E26" s="7">
+        <f t="shared" si="0"/>
+        <v>18.992379210486213</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="str">
+        <v>Finis Valorum</v>
+      </c>
+      <c r="C27">
+        <v>170</v>
+      </c>
+      <c r="D27" s="7">
+        <f>$H$12-$C27</f>
+        <v>4.3580246913580254</v>
+      </c>
+      <c r="E27" s="7">
+        <f t="shared" si="0"/>
+        <v>18.992379210486213</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="str">
+        <v>Luminara Unduli</v>
+      </c>
+      <c r="C28">
+        <v>170</v>
+      </c>
+      <c r="D28" s="7">
+        <f>$H$12-$C28</f>
+        <v>4.3580246913580254</v>
+      </c>
+      <c r="E28" s="7">
+        <f t="shared" si="0"/>
+        <v>18.992379210486213</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="str">
+        <v>Eeth Koth</v>
+      </c>
+      <c r="C29">
+        <v>171</v>
+      </c>
+      <c r="D29" s="7">
+        <f>$H$12-$C29</f>
+        <v>3.3580246913580254</v>
+      </c>
+      <c r="E29" s="7">
+        <f t="shared" si="0"/>
+        <v>11.276329827770162</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="str">
+        <v>Luke Skywalker</v>
+      </c>
+      <c r="C30">
+        <v>172</v>
+      </c>
+      <c r="D30" s="7">
+        <f>$H$12-$C30</f>
+        <v>2.3580246913580254</v>
+      </c>
+      <c r="E30" s="7">
+        <f t="shared" si="0"/>
+        <v>5.5602804450541106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="str">
+        <v>Greedo</v>
+      </c>
+      <c r="C31">
+        <v>173</v>
+      </c>
+      <c r="D31" s="7">
+        <f>$H$12-$C31</f>
+        <v>1.3580246913580254</v>
+      </c>
+      <c r="E31" s="7">
+        <f t="shared" si="0"/>
+        <v>1.8442310623380602</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="str">
+        <v>Jabba Desilijic Tiure</v>
+      </c>
+      <c r="C32">
+        <v>175</v>
+      </c>
+      <c r="D32" s="7">
+        <f>$H$12-$C32</f>
+        <v>-0.64197530864197461</v>
+      </c>
+      <c r="E32" s="7">
+        <f t="shared" si="0"/>
+        <v>0.41213229690595854</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="str">
+        <v>Lobot</v>
+      </c>
+      <c r="C33">
+        <v>175</v>
+      </c>
+      <c r="D33" s="7">
+        <f>$H$12-$C33</f>
+        <v>-0.64197530864197461</v>
+      </c>
+      <c r="E33" s="7">
+        <f t="shared" si="0"/>
+        <v>0.41213229690595854</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="str">
+        <v>Darth Maul</v>
+      </c>
+      <c r="C34">
+        <v>175</v>
+      </c>
+      <c r="D34" s="7">
+        <f>$H$12-$C34</f>
+        <v>-0.64197530864197461</v>
+      </c>
+      <c r="E34" s="7">
+        <f t="shared" si="0"/>
+        <v>0.41213229690595854</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="str">
+        <v>Lando Calrissian</v>
+      </c>
+      <c r="C35">
+        <v>177</v>
+      </c>
+      <c r="D35" s="7">
+        <f>$H$12-$C35</f>
+        <v>-2.6419753086419746</v>
+      </c>
+      <c r="E35" s="7">
+        <f t="shared" si="0"/>
+        <v>6.9800335314738566</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="str">
+        <v>Owen Lars</v>
+      </c>
+      <c r="C36">
+        <v>178</v>
+      </c>
+      <c r="D36" s="7">
+        <f>$H$12-$C36</f>
+        <v>-3.6419753086419746</v>
+      </c>
+      <c r="E36" s="7">
+        <f t="shared" si="0"/>
+        <v>13.263984148757807</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="str">
+        <v>Ayla Secura</v>
+      </c>
+      <c r="C37">
+        <v>178</v>
+      </c>
+      <c r="D37" s="7">
+        <f>$H$12-$C37</f>
+        <v>-3.6419753086419746</v>
+      </c>
+      <c r="E37" s="7">
+        <f t="shared" si="0"/>
+        <v>13.263984148757807</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Shaak Ti</v>
+      </c>
+      <c r="C38">
+        <v>178</v>
+      </c>
+      <c r="D38" s="7">
+        <f>$H$12-$C38</f>
+        <v>-3.6419753086419746</v>
+      </c>
+      <c r="E38" s="7">
+        <f t="shared" si="0"/>
+        <v>13.263984148757807</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="str">
+        <v>Sly Moore</v>
+      </c>
+      <c r="C39">
+        <v>178</v>
+      </c>
+      <c r="D39" s="7">
+        <f>$H$12-$C39</f>
+        <v>-3.6419753086419746</v>
+      </c>
+      <c r="E39" s="7">
+        <f t="shared" si="0"/>
+        <v>13.263984148757807</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="str">
+        <v>Wilhuff Tarkin</v>
+      </c>
+      <c r="C40">
+        <v>180</v>
+      </c>
+      <c r="D40" s="7">
+        <f>$H$12-$C40</f>
+        <v>-5.6419753086419746</v>
+      </c>
+      <c r="E40" s="7">
+        <f t="shared" si="0"/>
+        <v>31.831885383325705</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="str">
+        <v>Han Solo</v>
+      </c>
+      <c r="C41">
+        <v>180</v>
+      </c>
+      <c r="D41" s="7">
+        <f>$H$12-$C41</f>
+        <v>-5.6419753086419746</v>
+      </c>
+      <c r="E41" s="7">
+        <f t="shared" si="0"/>
+        <v>31.831885383325705</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="str">
+        <v>Jek Tono Porkins</v>
+      </c>
+      <c r="C42">
+        <v>180</v>
+      </c>
+      <c r="D42" s="7">
+        <f>$H$12-$C42</f>
+        <v>-5.6419753086419746</v>
+      </c>
+      <c r="E42" s="7">
+        <f t="shared" si="0"/>
+        <v>31.831885383325705</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="str">
+        <v>Ackbar</v>
+      </c>
+      <c r="C43">
+        <v>180</v>
+      </c>
+      <c r="D43" s="7">
+        <f>$H$12-$C43</f>
+        <v>-5.6419753086419746</v>
+      </c>
+      <c r="E43" s="7">
+        <f t="shared" si="0"/>
+        <v>31.831885383325705</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="str">
+        <v>Bib Fortuna</v>
+      </c>
+      <c r="C44">
+        <v>180</v>
+      </c>
+      <c r="D44" s="7">
+        <f>$H$12-$C44</f>
+        <v>-5.6419753086419746</v>
+      </c>
+      <c r="E44" s="7">
+        <f t="shared" si="0"/>
+        <v>31.831885383325705</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="str">
+        <v>Obi-Wan Kenobi</v>
+      </c>
+      <c r="C45">
+        <v>182</v>
+      </c>
+      <c r="D45" s="7">
+        <f>$H$12-$C45</f>
+        <v>-7.6419753086419746</v>
+      </c>
+      <c r="E45" s="7">
+        <f t="shared" si="0"/>
+        <v>58.399786617893604</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="str">
+        <v>Biggs Darklighter</v>
+      </c>
+      <c r="C46">
+        <v>183</v>
+      </c>
+      <c r="D46" s="7">
+        <f>$H$12-$C46</f>
+        <v>-8.6419753086419746</v>
+      </c>
+      <c r="E46" s="7">
+        <f t="shared" si="0"/>
+        <v>74.683737235177546</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="str">
+        <v>Boba Fett</v>
+      </c>
+      <c r="C47">
+        <v>183</v>
+      </c>
+      <c r="D47" s="7">
+        <f>$H$12-$C47</f>
+        <v>-8.6419753086419746</v>
+      </c>
+      <c r="E47" s="7">
+        <f t="shared" si="0"/>
+        <v>74.683737235177546</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="str">
+        <v>Ric Olié</v>
+      </c>
+      <c r="C48">
+        <v>183</v>
+      </c>
+      <c r="D48" s="7">
+        <f>$H$12-$C48</f>
+        <v>-8.6419753086419746</v>
+      </c>
+      <c r="E48" s="7">
+        <f t="shared" si="0"/>
+        <v>74.683737235177546</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="str">
+        <v>Quarsh Panaka</v>
+      </c>
+      <c r="C49">
+        <v>183</v>
+      </c>
+      <c r="D49" s="7">
+        <f>$H$12-$C49</f>
+        <v>-8.6419753086419746</v>
+      </c>
+      <c r="E49" s="7">
+        <f t="shared" si="0"/>
+        <v>74.683737235177546</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="str">
+        <v>Cliegg Lars</v>
+      </c>
+      <c r="C50">
+        <v>183</v>
+      </c>
+      <c r="D50" s="7">
+        <f>$H$12-$C50</f>
+        <v>-8.6419753086419746</v>
+      </c>
+      <c r="E50" s="7">
+        <f t="shared" si="0"/>
+        <v>74.683737235177546</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="str">
+        <v>Poggle the Lesser</v>
+      </c>
+      <c r="C51">
+        <v>183</v>
+      </c>
+      <c r="D51" s="7">
+        <f>$H$12-$C51</f>
+        <v>-8.6419753086419746</v>
+      </c>
+      <c r="E51" s="7">
+        <f t="shared" si="0"/>
+        <v>74.683737235177546</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="str">
+        <v>Jango Fett</v>
+      </c>
+      <c r="C52">
+        <v>183</v>
+      </c>
+      <c r="D52" s="7">
+        <f>$H$12-$C52</f>
+        <v>-8.6419753086419746</v>
+      </c>
+      <c r="E52" s="7">
+        <f t="shared" si="0"/>
+        <v>74.683737235177546</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="str">
+        <v>Adi Gallia</v>
+      </c>
+      <c r="C53">
+        <v>184</v>
+      </c>
+      <c r="D53" s="7">
+        <f>$H$12-$C53</f>
+        <v>-9.6419753086419746</v>
+      </c>
+      <c r="E53" s="7">
+        <f t="shared" si="0"/>
+        <v>92.967687852461495</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="str">
+        <v>Gregar Typho</v>
+      </c>
+      <c r="C54">
+        <v>185</v>
+      </c>
+      <c r="D54" s="7">
+        <f>$H$12-$C54</f>
+        <v>-10.641975308641975</v>
+      </c>
+      <c r="E54" s="7">
+        <f t="shared" si="0"/>
+        <v>113.25163846974544</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="str">
+        <v>Anakin Skywalker</v>
+      </c>
+      <c r="C55">
+        <v>188</v>
+      </c>
+      <c r="D55" s="7">
+        <f>$H$12-$C55</f>
+        <v>-13.641975308641975</v>
+      </c>
+      <c r="E55" s="7">
+        <f t="shared" si="0"/>
+        <v>186.10349032159729</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="str">
+        <v>Mace Windu</v>
+      </c>
+      <c r="C56">
+        <v>188</v>
+      </c>
+      <c r="D56" s="7">
+        <f>$H$12-$C56</f>
+        <v>-13.641975308641975</v>
+      </c>
+      <c r="E56" s="7">
+        <f t="shared" si="0"/>
+        <v>186.10349032159729</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="str">
+        <v>Saesee Tiin</v>
+      </c>
+      <c r="C57">
+        <v>188</v>
+      </c>
+      <c r="D57" s="7">
+        <f>$H$12-$C57</f>
+        <v>-13.641975308641975</v>
+      </c>
+      <c r="E57" s="7">
+        <f t="shared" si="0"/>
+        <v>186.10349032159729</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="str">
+        <v>Plo Koon</v>
+      </c>
+      <c r="C58">
+        <v>188</v>
+      </c>
+      <c r="D58" s="7">
+        <f>$H$12-$C58</f>
+        <v>-13.641975308641975</v>
+      </c>
+      <c r="E58" s="7">
+        <f t="shared" si="0"/>
+        <v>186.10349032159729</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="str">
+        <v>Raymus Antilles</v>
+      </c>
+      <c r="C59">
+        <v>188</v>
+      </c>
+      <c r="D59" s="7">
+        <f>$H$12-$C59</f>
+        <v>-13.641975308641975</v>
+      </c>
+      <c r="E59" s="7">
+        <f t="shared" si="0"/>
+        <v>186.10349032159729</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="str">
+        <v>Bossk</v>
+      </c>
+      <c r="C60">
+        <v>190</v>
+      </c>
+      <c r="D60" s="7">
+        <f>$H$12-$C60</f>
+        <v>-15.641975308641975</v>
+      </c>
+      <c r="E60" s="7">
+        <f t="shared" si="0"/>
+        <v>244.67139155616519</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="str">
+        <v>Nute Gunray</v>
+      </c>
+      <c r="C61">
+        <v>191</v>
+      </c>
+      <c r="D61" s="7">
+        <f>$H$12-$C61</f>
+        <v>-16.641975308641975</v>
+      </c>
+      <c r="E61" s="7">
+        <f t="shared" si="0"/>
+        <v>276.95534217344914</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="str">
+        <v>Bail Prestor Organa</v>
+      </c>
+      <c r="C62">
+        <v>191</v>
+      </c>
+      <c r="D62" s="7">
+        <f>$H$12-$C62</f>
+        <v>-16.641975308641975</v>
+      </c>
+      <c r="E62" s="7">
+        <f t="shared" si="0"/>
+        <v>276.95534217344914</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="str">
+        <v>San Hill</v>
+      </c>
+      <c r="C63">
+        <v>191</v>
+      </c>
+      <c r="D63" s="7">
+        <f>$H$12-$C63</f>
+        <v>-16.641975308641975</v>
+      </c>
+      <c r="E63" s="7">
+        <f t="shared" si="0"/>
+        <v>276.95534217344914</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="str">
+        <v>Qui-Gon Jinn</v>
+      </c>
+      <c r="C64">
+        <v>193</v>
+      </c>
+      <c r="D64" s="7">
+        <f>$H$12-$C64</f>
+        <v>-18.641975308641975</v>
+      </c>
+      <c r="E64" s="7">
+        <f t="shared" si="0"/>
+        <v>347.52324340801704</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="str">
+        <v>Dooku</v>
+      </c>
+      <c r="C65">
+        <v>193</v>
+      </c>
+      <c r="D65" s="7">
+        <f>$H$12-$C65</f>
+        <v>-18.641975308641975</v>
+      </c>
+      <c r="E65" s="7">
+        <f t="shared" si="0"/>
+        <v>347.52324340801704</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="str">
+        <v>Wat Tambor</v>
+      </c>
+      <c r="C66">
+        <v>193</v>
+      </c>
+      <c r="D66" s="7">
+        <f>$H$12-$C66</f>
+        <v>-18.641975308641975</v>
+      </c>
+      <c r="E66" s="7">
+        <f t="shared" si="0"/>
+        <v>347.52324340801704</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="str">
+        <v>Jar Jar Binks</v>
+      </c>
+      <c r="C67">
+        <v>196</v>
+      </c>
+      <c r="D67" s="7">
+        <f>$H$12-$C67</f>
+        <v>-21.641975308641975</v>
+      </c>
+      <c r="E67" s="7">
+        <f t="shared" ref="E67:E82" si="1">$D67^2</f>
+        <v>468.37509525986889</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="str">
+        <v>Kit Fisto</v>
+      </c>
+      <c r="C68">
+        <v>196</v>
+      </c>
+      <c r="D68" s="7">
+        <f>$H$12-$C68</f>
+        <v>-21.641975308641975</v>
+      </c>
+      <c r="E68" s="7">
+        <f t="shared" si="1"/>
+        <v>468.37509525986889</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="str">
+        <v>Mas Amedda</v>
+      </c>
+      <c r="C69">
+        <v>196</v>
+      </c>
+      <c r="D69" s="7">
+        <f>$H$12-$C69</f>
+        <v>-21.641975308641975</v>
+      </c>
+      <c r="E69" s="7">
+        <f t="shared" si="1"/>
+        <v>468.37509525986889</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="str">
+        <v>Ki-Adi-Mundi</v>
+      </c>
+      <c r="C70">
+        <v>198</v>
+      </c>
+      <c r="D70" s="7">
+        <f>$H$12-$C70</f>
+        <v>-23.641975308641975</v>
+      </c>
+      <c r="E70" s="7">
+        <f t="shared" si="1"/>
+        <v>558.94299649443678</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="str">
+        <v>Dexter Jettster</v>
+      </c>
+      <c r="C71">
+        <v>198</v>
+      </c>
+      <c r="D71" s="7">
+        <f>$H$12-$C71</f>
+        <v>-23.641975308641975</v>
+      </c>
+      <c r="E71" s="7">
+        <f t="shared" si="1"/>
+        <v>558.94299649443678</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="str">
+        <v>IG-88</v>
+      </c>
+      <c r="C72">
+        <v>200</v>
+      </c>
+      <c r="D72" s="7">
+        <f>$H$12-$C72</f>
+        <v>-25.641975308641975</v>
+      </c>
+      <c r="E72" s="7">
+        <f t="shared" si="1"/>
+        <v>657.51089772900468</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="str">
+        <v>Darth Vader</v>
+      </c>
+      <c r="C73">
+        <v>202</v>
+      </c>
+      <c r="D73" s="7">
+        <f>$H$12-$C73</f>
+        <v>-27.641975308641975</v>
+      </c>
+      <c r="E73" s="7">
+        <f t="shared" si="1"/>
+        <v>764.07879896357258</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="str">
+        <v>Rugor Nass</v>
+      </c>
+      <c r="C74">
+        <v>206</v>
+      </c>
+      <c r="D74" s="7">
+        <f>$H$12-$C74</f>
+        <v>-31.641975308641975</v>
+      </c>
+      <c r="E74" s="7">
+        <f t="shared" si="1"/>
+        <v>1001.2146014327084</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="str">
+        <v>Tion Medon</v>
+      </c>
+      <c r="C75">
+        <v>206</v>
+      </c>
+      <c r="D75" s="7">
+        <f>$H$12-$C75</f>
+        <v>-31.641975308641975</v>
+      </c>
+      <c r="E75" s="7">
+        <f t="shared" si="1"/>
+        <v>1001.2146014327084</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="str">
+        <v>Taun We</v>
+      </c>
+      <c r="C76">
+        <v>213</v>
+      </c>
+      <c r="D76" s="7">
+        <f>$H$12-$C76</f>
+        <v>-38.641975308641975</v>
+      </c>
+      <c r="E76" s="7">
+        <f t="shared" si="1"/>
+        <v>1493.2022557536961</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="str">
+        <v>Grievous</v>
+      </c>
+      <c r="C77">
+        <v>216</v>
+      </c>
+      <c r="D77" s="7">
+        <f>$H$12-$C77</f>
+        <v>-41.641975308641975</v>
+      </c>
+      <c r="E77" s="7">
+        <f t="shared" si="1"/>
+        <v>1734.0541076055479</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="str">
+        <v>Roos Tarpals</v>
+      </c>
+      <c r="C78">
+        <v>224</v>
+      </c>
+      <c r="D78" s="7">
+        <f>$H$12-$C78</f>
+        <v>-49.641975308641975</v>
+      </c>
+      <c r="E78" s="7">
+        <f t="shared" si="1"/>
+        <v>2464.3257125438195</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="str">
+        <v>Chewbacca</v>
+      </c>
+      <c r="C79">
+        <v>228</v>
+      </c>
+      <c r="D79" s="7">
+        <f>$H$12-$C79</f>
+        <v>-53.641975308641975</v>
+      </c>
+      <c r="E79" s="7">
+        <f t="shared" si="1"/>
+        <v>2877.4615150129553</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="str">
+        <v>Lama Su</v>
+      </c>
+      <c r="C80">
+        <v>229</v>
+      </c>
+      <c r="D80" s="7">
+        <f>$H$12-$C80</f>
+        <v>-54.641975308641975</v>
+      </c>
+      <c r="E80" s="7">
+        <f t="shared" si="1"/>
+        <v>2985.7454656302393</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="str">
+        <v>Tarfful</v>
+      </c>
+      <c r="C81">
+        <v>234</v>
+      </c>
+      <c r="D81" s="7">
+        <f>$H$12-$C81</f>
+        <v>-59.641975308641975</v>
+      </c>
+      <c r="E81" s="7">
+        <f t="shared" si="1"/>
+        <v>3557.1652187166592</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="str">
+        <v>Yarael Poof</v>
+      </c>
+      <c r="C82">
+        <v>264</v>
+      </c>
+      <c r="D82" s="7">
+        <f>$H$12-$C82</f>
+        <v>-89.641975308641975</v>
+      </c>
+      <c r="E82" s="7">
+        <f t="shared" si="1"/>
+        <v>8035.6837372351774</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C83:E1048576 C1:C82">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C9AD6C-192F-4898-AF47-D19C02D8C3A5}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -8198,7 +10008,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E3A0F5D-FDF8-4BF8-BD72-0610A843EBFA}">
   <dimension ref="A1:B10"/>
   <sheetViews>

</xml_diff>